<commit_message>
AIP-1228 AIP-1275 Written code for enabling IEC61850 and then trying to connect with IECBrwoser using all cablings
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_792.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_792.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAB47CD-5488-49BC-AE12-60F06B924186}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1AD765-FBB7-432D-91AE-96D35FBE1136}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,16 +46,16 @@
     <t>DeviceIPAdd</t>
   </si>
   <si>
-    <t>10.75.58.53</t>
-  </si>
-  <si>
     <t>Protocol_Name</t>
   </si>
   <si>
     <t>IEC 61850 Ed1</t>
   </si>
   <si>
-    <t>IND_DAU_53</t>
+    <t>IND_DAU_51</t>
+  </si>
+  <si>
+    <t>10.75.58.51</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,7 +412,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -423,19 +423,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1">
         <v>409026540</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AIP-1228 AIP-1275 Written code for checking the Prototcol is up or not in the device
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_792.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_792.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1AD765-FBB7-432D-91AE-96D35FBE1136}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D066E9F0-933A-468A-A8F2-813F7610AF1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,19 +380,19 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -415,7 +415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Updated MDS file for master merge and one test data file for updating test code
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_792.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_792.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D066E9F0-933A-468A-A8F2-813F7610AF1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B7F1BC-2EE9-4DE1-81CE-B86F778BE6C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,13 +49,13 @@
     <t>Protocol_Name</t>
   </si>
   <si>
-    <t>IEC 61850 Ed1</t>
-  </si>
-  <si>
     <t>IND_DAU_51</t>
   </si>
   <si>
     <t>10.75.58.51</t>
+  </si>
+  <si>
+    <t>IEC 61850 Ed2</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,19 +423,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1">
         <v>409026540</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>